<commit_message>
vẽ xong thẻ sửa cấu trúc Study
</commit_message>
<xml_diff>
--- a/src/data/dataFile/xlsx/family.xlsx
+++ b/src/data/dataFile/xlsx/family.xlsx
@@ -1,32 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Java\Dictionary\src\resrc\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\java\Dictionary\src\data\dataFile\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>gia đình</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Tieng Viet</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>great-grandparent</t>
+  </si>
+  <si>
+    <t>ông bà cố</t>
+  </si>
+  <si>
+    <t>nothing</t>
+  </si>
+  <si>
+    <t>grandmother</t>
+  </si>
+  <si>
+    <t>bà </t>
   </si>
   <si>
     <t>ancestor</t>
@@ -35,72 +51,41 @@
     <t>tổ tiên</t>
   </si>
   <si>
-    <t>ông bà cố</t>
+    <t>grandfather</t>
   </si>
   <si>
     <t>ông (nội, ngoại)</t>
   </si>
   <si>
-    <t>bà </t>
+    <t>family</t>
+  </si>
+  <si>
+    <t>brother</t>
   </si>
   <si>
     <t>anh/em trai ruột</t>
   </si>
   <si>
+    <t>sister</t>
+  </si>
+  <si>
     <t>chị/em gái ruột</t>
   </si>
   <si>
-    <t>brother</t>
-  </si>
-  <si>
-    <t>grandmother</t>
-  </si>
-  <si>
-    <t>sister</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grandfather  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">family </t>
-  </si>
-  <si>
-    <t xml:space="preserve">great-grandparent  </t>
-  </si>
-  <si>
-    <t>E:\Java\Dictionary\src\resrc\img\anh, the gioi va em.jpg</t>
-  </si>
-  <si>
-    <t>E:\Java\Dictionary\src\resrc\img\Autumn.jpg</t>
-  </si>
-  <si>
-    <t>E:\Java\Dictionary\src\resrc\img\nguoc.jpg</t>
+    <t>gia đình fsjg ofjdp sdpjfpjdsafpsap fsfosdfpsd fpspfospofkspfkposdkfpjgpjsg s jgposjfpsjdfpafs o sf sf sdf s fspjfpu09wf09asjf sdfw fs f jsa0fjw0 fjsdf jawf sa0 fjwejf 0sf afp jasd;fja; fa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Verdana"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -123,10 +108,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,107 +423,104 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="2" width="36.85546875" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
flashcard ko nhận word từ manager. Buồn ngủ
</commit_message>
<xml_diff>
--- a/src/data/dataFile/xlsx/family.xlsx
+++ b/src/data/dataFile/xlsx/family.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>English</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>gia đình fsjg ofjdp sdpjfpjdsafpsap fsfosdfpsd fpspfospofkspfkposdkfpjgpjsg s jgposjfpsjdfpafs o sf sf sdf s fspjfpu09wf09asjf sdfw fs f jsa0fjw0 fjsdf jawf sa0 fjwejf 0sf afp jasd;fja; fa</t>
+  </si>
+  <si>
+    <t>hard</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,7 +454,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -462,7 +465,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -495,7 +498,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Sửa xong cái Search với xóa từ trong GroupManager
</commit_message>
<xml_diff>
--- a/src/data/dataFile/xlsx/family.xlsx
+++ b/src/data/dataFile/xlsx/family.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>English</t>
   </si>
@@ -42,12 +42,6 @@
   </si>
   <si>
     <t>bà </t>
-  </si>
-  <si>
-    <t>ancestor</t>
-  </si>
-  <si>
-    <t>tổ tiên</t>
   </si>
   <si>
     <t>grandfather</t>
@@ -172,7 +166,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -180,13 +174,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -200,23 +194,9 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>